<commit_message>
Update circ by borrower files for January 2023
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.d.monthly_circ_by_borrower.zipcode.xlsx
+++ b/statistics_files/2023/2023.d.monthly_circ_by_borrower.zipcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FAB0C9-FC46-4E4C-92A9-7FBDA905FE07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E83240-46FC-46DF-82F7-17295D5CA66C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11390" tabRatio="894" firstSheet="1" activeTab="1" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
   </bookViews>
@@ -648,6 +648,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{7C32E5BA-FB02-42A6-81B1-F4CE0BD47B44}"/>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A &quot;-&quot; indicates zip codes that have been anonymized." sqref="B1" xr:uid="{1DE16DDD-4058-45A8-BA24-0FEEC25CF001}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -701,6 +704,9 @@
     <sortCondition ref="A2:A712"/>
     <sortCondition ref="B2:B712"/>
   </sortState>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A &quot;-&quot; indicates zip codes that have been anonymized." sqref="B1" xr:uid="{C802CE93-E6EF-46B4-9763-C3800FBF168B}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -750,6 +756,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{56A1A629-CA91-47DF-B266-9A81672C9993}"/>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A &quot;-&quot; indicates zip codes that have been anonymized." sqref="B1" xr:uid="{E72413A1-6D99-4165-A4A6-1A894F2AA13F}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -803,6 +812,9 @@
     <sortCondition ref="A2:A744"/>
     <sortCondition ref="B2:B744"/>
   </sortState>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A &quot;-&quot; indicates zip codes that have been anonymized." sqref="B1" xr:uid="{8DF1027C-E14C-4157-B8D3-524BF6C91B46}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -856,6 +868,9 @@
     <sortCondition ref="A2:A685"/>
     <sortCondition ref="B2:B685"/>
   </sortState>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A &quot;-&quot; indicates zip codes that have been anonymized." sqref="B1" xr:uid="{1E057445-5840-4C57-AD8A-1E16505F1AF2}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -882,7 +897,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8662,7 +8677,7 @@
     </sortState>
   </autoFilter>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A &quot;-&quot; indicates that those zip codes have been anonymized because that zip code is used by fewer than 10 borrowers system-wide." sqref="B1" xr:uid="{D92B399E-F56A-4EF7-A3CB-B138F4765858}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A &quot;-&quot; indicates zip codes that have been anonymized." sqref="B1" xr:uid="{D92B399E-F56A-4EF7-A3CB-B138F4765858}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8704,6 +8719,9 @@
     <sortCondition ref="A2:A696"/>
     <sortCondition ref="B2:B696"/>
   </sortState>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A &quot;-&quot; indicates zip codes that have been anonymized." sqref="B1" xr:uid="{5FB4A901-E50F-4CE3-9562-51251A274DBD}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8757,6 +8775,9 @@
     <sortCondition ref="A2:A674"/>
     <sortCondition ref="B2:B674"/>
   </sortState>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A &quot;-&quot; indicates zip codes that have been anonymized." sqref="B1" xr:uid="{9DACE48B-FBDA-410B-AC57-A77707C52B74}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8781,8 +8802,9 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
+      <selection sqref="A1:C1"/>
+      <selection pane="topRight" sqref="A1:C1"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -8806,6 +8828,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{39260CD5-B183-4F8E-B865-E4FCFB0FCA98}"/>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A &quot;-&quot; indicates zip codes that have been anonymized." sqref="B1" xr:uid="{7AD32CEF-7EEE-4F66-A8DB-CFA4E4E354DB}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8872,6 +8897,9 @@
     <sortCondition ref="A2:A648"/>
     <sortCondition ref="B2:B648"/>
   </sortState>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A &quot;-&quot; indicates zip codes that have been anonymized." sqref="B1" xr:uid="{DAD1236B-34AE-448B-9419-ABA54A9A69FA}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8925,6 +8953,9 @@
     <sortCondition ref="A2:A720"/>
     <sortCondition ref="B2:B720"/>
   </sortState>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A &quot;-&quot; indicates zip codes that have been anonymized." sqref="B1" xr:uid="{8592973C-1C53-4C03-A3A3-C3120BF1DA69}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8974,6 +9005,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{419F4E40-BF52-4D5C-8BEF-0CD3CC7A9C4F}"/>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A &quot;-&quot; indicates zip codes that have been anonymized." sqref="B1" xr:uid="{D75C5898-6933-409C-8625-FC4E49751A45}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>